<commit_message>
Update code tes parameter kalman
</commit_message>
<xml_diff>
--- a/Data Penelitian/Pengujian Keempat/2.4Ghz/VisualisasiData4-(2,4Ghz).xlsx
+++ b/Data Penelitian/Pengujian Keempat/2.4Ghz/VisualisasiData4-(2,4Ghz).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fathan Firmansyah\Desktop\TES\Data Penelitian\Pengujian Keempat\2.4Ghz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02475708-395D-42EE-9633-C070782A7B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7339FA01-26CD-461E-ABA0-A5F38B8EE979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E3C1A04C-9372-4545-A9E6-98ACBC17DC40}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E3C1A04C-9372-4545-A9E6-98ACBC17DC40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,7 +108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -116,6 +116,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5596,7 +5597,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{066A4C68-0146-494E-97F7-39A23A79B518}" name="Table2" displayName="Table2" ref="H2:K35" totalsRowShown="0">
   <autoFilter ref="H2:K35" xr:uid="{066A4C68-0146-494E-97F7-39A23A79B518}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{54DB678F-606C-462F-BE97-03026FCC50EE}" name="Target" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{54DB678F-606C-462F-BE97-03026FCC50EE}" name="Target" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{681602B0-EA1F-4949-8167-35C558E06C56}" name="RSSI"/>
     <tableColumn id="3" xr3:uid="{01F7D8C4-4585-4EFE-A279-53EA846111F6}" name="No Filter"/>
     <tableColumn id="4" xr3:uid="{5886D9EC-332E-477A-A555-7BE04B78DD8A}" name="Kalman Filter"/>
@@ -5606,39 +5607,39 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{537E818B-5994-4840-8147-34EAD963A7D0}" name="Table3" displayName="Table3" ref="M2:P35" totalsRowShown="0" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{537E818B-5994-4840-8147-34EAD963A7D0}" name="Table3" displayName="Table3" ref="M2:P35" totalsRowShown="0" dataDxfId="15">
   <autoFilter ref="M2:P35" xr:uid="{537E818B-5994-4840-8147-34EAD963A7D0}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{FE3FBC5E-5F4A-40AF-823F-2E65B3FD313E}" name="Target" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{FAF18BAE-54C8-460A-B2A2-EC501824E2FA}" name="RSSI" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{F35E2D5D-D422-45E1-A031-FB42D924B0AC}" name="No Filter" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{F797CC7F-83C5-42E8-AB4A-DFD463179C75}" name="Kalman Filter" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{FE3FBC5E-5F4A-40AF-823F-2E65B3FD313E}" name="Target" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{FAF18BAE-54C8-460A-B2A2-EC501824E2FA}" name="RSSI" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{F35E2D5D-D422-45E1-A031-FB42D924B0AC}" name="No Filter" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{F797CC7F-83C5-42E8-AB4A-DFD463179C75}" name="Kalman Filter" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{6E854493-1F3E-4D9A-8C92-936D1F6590ED}" name="Table4" displayName="Table4" ref="R2:U35" totalsRowShown="0" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{6E854493-1F3E-4D9A-8C92-936D1F6590ED}" name="Table4" displayName="Table4" ref="R2:U35" totalsRowShown="0" dataDxfId="10">
   <autoFilter ref="R2:U35" xr:uid="{6E854493-1F3E-4D9A-8C92-936D1F6590ED}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E7C8A689-03F4-44EE-A0CE-C55599EE1067}" name="Target" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{411BBD40-E490-4959-918A-E9007B605795}" name="RSSI" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{8395C691-C43B-4D44-B86D-26F43AE177FE}" name="No Filter" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{75EAB1DF-CF92-4D81-B0E9-FD5B1D8969BD}" name="Kalman Filter" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{E7C8A689-03F4-44EE-A0CE-C55599EE1067}" name="Target" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{411BBD40-E490-4959-918A-E9007B605795}" name="RSSI" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{8395C691-C43B-4D44-B86D-26F43AE177FE}" name="No Filter" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{75EAB1DF-CF92-4D81-B0E9-FD5B1D8969BD}" name="Kalman Filter" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{B72A6723-0602-496E-9742-77D19D50EF8B}" name="Table5" displayName="Table5" ref="W2:Z35" totalsRowShown="0" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{B72A6723-0602-496E-9742-77D19D50EF8B}" name="Table5" displayName="Table5" ref="W2:Z35" totalsRowShown="0" dataDxfId="5">
   <autoFilter ref="W2:Z35" xr:uid="{B72A6723-0602-496E-9742-77D19D50EF8B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{75D3AFDA-CDC5-4060-BA7A-64E5CEECB5D1}" name="Target" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{21F2121F-8C84-47ED-8843-A9D2891326F0}" name="RSSI" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{CCF10C6E-E5D1-4C57-887C-4422EF11C0C2}" name="No Filter" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{B80B4DCF-3EBA-42A7-92B3-2B8957BC727D}" name="Kalman Filter" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{75D3AFDA-CDC5-4060-BA7A-64E5CEECB5D1}" name="Target" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{21F2121F-8C84-47ED-8843-A9D2891326F0}" name="RSSI" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{CCF10C6E-E5D1-4C57-887C-4422EF11C0C2}" name="No Filter" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{B80B4DCF-3EBA-42A7-92B3-2B8957BC727D}" name="Kalman Filter" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5941,39 +5942,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC04783-8983-41FB-874F-D304B1E277AA}">
-  <dimension ref="C1:Z35"/>
+  <dimension ref="C1:Z52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V18" sqref="V18"/>
+    <sheetView tabSelected="1" topLeftCell="I27" zoomScale="85" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q53" sqref="Q53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" customWidth="1"/>
-    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="15" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:26" x14ac:dyDescent="0.3">
       <c r="I1" t="s">
         <v>0</v>
       </c>
@@ -5987,7 +5988,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>1</v>
       </c>
@@ -6049,7 +6050,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
       <c r="D3" s="1">
         <v>-26</v>
@@ -6109,7 +6110,7 @@
         <v>3.98</v>
       </c>
     </row>
-    <row r="4" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
       <c r="D4" s="1">
         <v>-26</v>
@@ -6170,7 +6171,7 @@
         <v>9.44</v>
       </c>
     </row>
-    <row r="5" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
       <c r="D5" s="1">
         <v>-33</v>
@@ -6231,7 +6232,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="6" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C6" s="1"/>
       <c r="D6" s="1">
         <v>-33</v>
@@ -6292,7 +6293,7 @@
         <v>7.38</v>
       </c>
     </row>
-    <row r="7" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C7" s="1"/>
       <c r="D7" s="1">
         <v>-34</v>
@@ -6353,7 +6354,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="8" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
       <c r="D8" s="1">
         <v>-28</v>
@@ -6414,7 +6415,7 @@
         <v>6.46</v>
       </c>
     </row>
-    <row r="9" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C9" s="1"/>
       <c r="D9" s="1">
         <v>-28</v>
@@ -6475,7 +6476,7 @@
         <v>6.37</v>
       </c>
     </row>
-    <row r="10" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>
       <c r="D10" s="1">
         <v>-29</v>
@@ -6536,7 +6537,7 @@
         <v>5.1100000000000003</v>
       </c>
     </row>
-    <row r="11" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C11" s="1"/>
       <c r="D11" s="1">
         <v>-29</v>
@@ -6597,7 +6598,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="12" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C12" s="1"/>
       <c r="D12" s="1">
         <v>-29</v>
@@ -6658,7 +6659,7 @@
         <v>4.8899999999999997</v>
       </c>
     </row>
-    <row r="13" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
       <c r="D13" s="1">
         <v>-26</v>
@@ -6719,7 +6720,7 @@
         <v>4.97</v>
       </c>
     </row>
-    <row r="14" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>
       <c r="D14" s="1">
         <v>-26</v>
@@ -6780,7 +6781,7 @@
         <v>4.99</v>
       </c>
     </row>
-    <row r="15" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C15" s="1"/>
       <c r="D15" s="1">
         <v>-26</v>
@@ -6841,7 +6842,7 @@
         <v>5.37</v>
       </c>
     </row>
-    <row r="16" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C16" s="1"/>
       <c r="D16" s="1">
         <v>-25</v>
@@ -6902,7 +6903,7 @@
         <v>5.53</v>
       </c>
     </row>
-    <row r="17" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C17" s="1"/>
       <c r="D17" s="1">
         <v>-31</v>
@@ -6963,7 +6964,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="18" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C18" s="1"/>
       <c r="D18" s="1">
         <v>-31</v>
@@ -7024,7 +7025,7 @@
         <v>5.08</v>
       </c>
     </row>
-    <row r="19" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C19" s="1"/>
       <c r="D19" s="1">
         <v>-31</v>
@@ -7085,7 +7086,7 @@
         <v>5.04</v>
       </c>
     </row>
-    <row r="20" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C20" s="1"/>
       <c r="D20" s="1">
         <v>-30</v>
@@ -7146,7 +7147,7 @@
         <v>4.68</v>
       </c>
     </row>
-    <row r="21" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C21" s="1"/>
       <c r="D21" s="1">
         <v>-30</v>
@@ -7207,7 +7208,7 @@
         <v>4.55</v>
       </c>
     </row>
-    <row r="22" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C22" s="1"/>
       <c r="D22" s="1">
         <v>-29</v>
@@ -7268,7 +7269,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="23" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
       <c r="D23" s="1">
         <v>-29</v>
@@ -7329,7 +7330,7 @@
         <v>5.16</v>
       </c>
     </row>
-    <row r="24" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C24" s="1"/>
       <c r="D24" s="1">
         <v>-29</v>
@@ -7389,7 +7390,7 @@
         <v>5.44</v>
       </c>
     </row>
-    <row r="25" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C25" s="1"/>
       <c r="D25" s="1">
         <v>-31</v>
@@ -7449,7 +7450,7 @@
         <v>5.55</v>
       </c>
     </row>
-    <row r="26" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C26" s="1"/>
       <c r="D26" s="1">
         <v>-31</v>
@@ -7509,7 +7510,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="27" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C27" s="1"/>
       <c r="D27" s="1">
         <v>-31</v>
@@ -7569,7 +7570,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="28" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C28" s="1"/>
       <c r="D28" s="1">
         <v>-28</v>
@@ -7629,7 +7630,7 @@
         <v>6.16</v>
       </c>
     </row>
-    <row r="29" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C29" s="1"/>
       <c r="D29" s="1">
         <v>-28</v>
@@ -7689,7 +7690,7 @@
         <v>5.42</v>
       </c>
     </row>
-    <row r="30" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C30" s="1"/>
       <c r="D30" s="1">
         <v>-31</v>
@@ -7749,7 +7750,7 @@
         <v>5.17</v>
       </c>
     </row>
-    <row r="31" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C31" s="1"/>
       <c r="D31" s="1">
         <v>-31</v>
@@ -7809,7 +7810,7 @@
         <v>5.07</v>
       </c>
     </row>
-    <row r="32" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C32" s="1"/>
       <c r="D32" s="1">
         <v>-31</v>
@@ -7869,7 +7870,7 @@
         <v>5.03</v>
       </c>
     </row>
-    <row r="33" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C33" s="1" t="s">
         <v>8</v>
       </c>
@@ -7934,7 +7935,7 @@
         <v>5.6679999999999984</v>
       </c>
     </row>
-    <row r="34" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C34" s="1" t="s">
         <v>10</v>
       </c>
@@ -7993,7 +7994,7 @@
         <v>0.66799999999999837</v>
       </c>
     </row>
-    <row r="35" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:26" x14ac:dyDescent="0.3">
       <c r="H35" s="1" t="s">
         <v>12</v>
       </c>
@@ -8030,6 +8031,58 @@
       </c>
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
+    </row>
+    <row r="51" spans="10:26" x14ac:dyDescent="0.3">
+      <c r="J51">
+        <f>STDEVP(J3:J32)</f>
+        <v>0.11800423721205799</v>
+      </c>
+      <c r="K51">
+        <f>STDEVP(K3:K32)</f>
+        <v>0.10242395553124355</v>
+      </c>
+      <c r="O51">
+        <f>_xlfn.STDEV.P(O3:O32)</f>
+        <v>0.12089665007765933</v>
+      </c>
+      <c r="P51">
+        <f>_xlfn.STDEV.P(P3:P32)</f>
+        <v>0.10654211478200637</v>
+      </c>
+      <c r="T51">
+        <f>_xlfn.STDEV.P(T3:T32)</f>
+        <v>0.87563570558131798</v>
+      </c>
+      <c r="U51">
+        <f>_xlfn.STDEV.P(U3:U32)</f>
+        <v>0.83801511521769434</v>
+      </c>
+      <c r="Y51">
+        <f>_xlfn.STDEV.P(Y3:Y32)</f>
+        <v>2.2656148540002699</v>
+      </c>
+      <c r="Z51">
+        <f>_xlfn.STDEV.P(Z3:Z32)</f>
+        <v>1.2230355677575422</v>
+      </c>
+    </row>
+    <row r="52" spans="10:26" x14ac:dyDescent="0.3">
+      <c r="J52" s="3">
+        <f>ABS(((K51-J51)/J51))</f>
+        <v>0.13203154436578496</v>
+      </c>
+      <c r="O52" s="3">
+        <f>ABS(((P51-O51)/O51))</f>
+        <v>0.11873393751135507</v>
+      </c>
+      <c r="T52" s="3">
+        <f>ABS(((U51-T51)/T51))</f>
+        <v>4.2963746366016499E-2</v>
+      </c>
+      <c r="Y52" s="3">
+        <f>ABS(((Z51-Y51)/Y51))</f>
+        <v>0.46017498711305832</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>